<commit_message>
Conclusão do trabalho de AED sobre ordenação
</commit_message>
<xml_diff>
--- a/AED/Algoritmos de ordenação/Planílha de comparação.xlsx
+++ b/AED/Algoritmos de ordenação/Planílha de comparação.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias.paiva\Desktop\Trabalhos_PUC\AED\Algoritmos de ordenação\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9780" activeTab="1"/>
   </bookViews>
@@ -15,9 +10,9 @@
     <sheet name="Gráf1" sheetId="2" r:id="rId1"/>
     <sheet name="Planilha1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -57,8 +52,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,22 +105,10 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -154,35 +137,24 @@
         </a:p>
       </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1158707279"/>
-        <c:axId val="1158709775"/>
+        <c:axId val="133344640"/>
+        <c:axId val="148632704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1158707279"/>
+        <c:axId val="133344640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -217,19 +189,17 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1158709775"/>
+        <c:crossAx val="148632704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1158709775"/>
+        <c:axId val="148632704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -246,7 +216,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -275,7 +244,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1158707279"/>
+        <c:crossAx val="133344640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -289,7 +258,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -320,18 +288,8 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -365,7 +323,6 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -373,34 +330,12 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -424,7 +359,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -456,14 +390,8 @@
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -544,7 +472,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000003B-6783-48CC-9102-FAE554ACBD63}"/>
             </c:ext>
@@ -573,7 +501,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -605,14 +532,8 @@
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -693,7 +614,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000003C-6783-48CC-9102-FAE554ACBD63}"/>
             </c:ext>
@@ -722,7 +643,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -754,14 +674,8 @@
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -842,7 +756,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000003D-6783-48CC-9102-FAE554ACBD63}"/>
             </c:ext>
@@ -871,7 +785,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -903,14 +816,8 @@
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -991,7 +898,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000003E-6783-48CC-9102-FAE554ACBD63}"/>
             </c:ext>
@@ -1020,7 +927,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -1052,14 +958,8 @@
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -1140,7 +1040,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000003F-6783-48CC-9102-FAE554ACBD63}"/>
             </c:ext>
@@ -1169,7 +1069,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -1201,14 +1100,8 @@
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showLeaderLines val="1"/>
@@ -1289,31 +1182,24 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000040-6783-48CC-9102-FAE554ACBD63}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
-          <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="1159606159"/>
-        <c:axId val="1159591183"/>
+        <c:axId val="149346176"/>
+        <c:axId val="149229568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1159606159"/>
+        <c:axId val="149346176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -1342,7 +1228,6 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1350,30 +1235,9 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1408,19 +1272,17 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1159591183"/>
+        <c:crossAx val="149229568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1159591183"/>
+        <c:axId val="149229568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1457,13 +1319,12 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-BR"/>
-                  <a:t>Tempo gasto no processamento (ms)</a:t>
+                  <a:t>Tempo gasto no processamento (s)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1471,30 +1332,9 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pt-BR"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1523,7 +1363,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1159606159"/>
+        <c:crossAx val="149346176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1538,7 +1378,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1569,7 +1408,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1598,7 +1436,2317 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000008" footer="0.31496062000000008"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Gráfico de desempenho</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> de ordenação de vetor ordenado crescente</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insert</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Planilha1!$B$2,Planilha1!$B$9,Planilha1!$B$16,Planilha1!$B$23,Planilha1!$B$30,Planilha1!$B$37,Planilha1!$B$44)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Planilha1!$E$3,Planilha1!$E$10,Planilha1!$E$17,Planilha1!$E$24,Planilha1!$E$31,Planilha1!$E$38,Planilha1!$E$45)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.0000000000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1333333333333335E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.19899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.73966666666666681</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7749999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.435333333333332</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000003B-6783-48CC-9102-FAE554ACBD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Select</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Planilha1!$B$2,Planilha1!$B$9,Planilha1!$B$16,Planilha1!$B$23,Planilha1!$B$30,Planilha1!$B$37,Planilha1!$B$44)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Planilha1!$I$4,Planilha1!$I$11,Planilha1!$I$18,Planilha1!$I$25,Planilha1!$I$32,Planilha1!$I$39,Planilha1!$I$46)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8000000000000009E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34766666666666662</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3966666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.6033333333333326</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.568000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000003C-6783-48CC-9102-FAE554ACBD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Planilha1!$B$2,Planilha1!$B$9,Planilha1!$B$16,Planilha1!$B$23,Planilha1!$B$30,Planilha1!$B$37,Planilha1!$B$44)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Planilha1!$I$5,Planilha1!$I$12,Planilha1!$I$19,Planilha1!$I$26,Planilha1!$I$33,Planilha1!$I$40,Planilha1!$I$47)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.1666666666666667E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9666666666666671E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.71799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.366999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>46.178666666666665</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000003D-6783-48CC-9102-FAE554ACBD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Merge</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Planilha1!$B$2,Planilha1!$B$9,Planilha1!$B$16,Planilha1!$B$23,Planilha1!$B$30,Planilha1!$B$37,Planilha1!$B$44)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Planilha1!$I$6,Planilha1!$I$13,Planilha1!$I$20,Planilha1!$I$27,Planilha1!$I$34,Planilha1!$I$41,Planilha1!$I$48)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1333333333333334E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.466666666666667E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000003E-6783-48CC-9102-FAE554ACBD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Planilha1!$B$2,Planilha1!$B$9,Planilha1!$B$16,Planilha1!$B$23,Planilha1!$B$30,Planilha1!$B$37,Planilha1!$B$44)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Planilha1!$I$7,Planilha1!$I$14,Planilha1!$I$21,Planilha1!$I$28,Planilha1!$I$35,Planilha1!$I$42,Planilha1!$I$49)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0000000000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000003F-6783-48CC-9102-FAE554ACBD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Select com bubble</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Planilha1!$B$2,Planilha1!$B$9,Planilha1!$B$16,Planilha1!$B$23,Planilha1!$B$30,Planilha1!$B$37,Planilha1!$B$44)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Planilha1!$I$8,Planilha1!$I$15,Planilha1!$I$22,Planilha1!$I$29,Planilha1!$I$36,Planilha1!$I$43,Planilha1!$I$50)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.3333333333333332E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2333333333333334E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34533333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3833333333333335</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.56</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.239000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000040-6783-48CC-9102-FAE554ACBD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="105895424"/>
+        <c:axId val="105897344"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="105895424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Quantidade de elementos no vetor</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="105897344"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="105897344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Tempo gasto no processamento (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="105895424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Gráfico de desempenho</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> de ordenação de vetor ordenado decrescente</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insert</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Planilha1!$B$2,Planilha1!$B$9,Planilha1!$B$16,Planilha1!$B$23,Planilha1!$B$30,Planilha1!$B$37,Planilha1!$B$44)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Planilha1!$M$3,Planilha1!$M$10,Planilha1!$M$17,Planilha1!$M$24,Planilha1!$M$31,Planilha1!$M$38,Planilha1!$M$45)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.6666666666666671E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3333333333333334E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.1000000000000011E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56966666666666665</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4749999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.927000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000003B-6783-48CC-9102-FAE554ACBD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Select</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Planilha1!$B$2,Planilha1!$B$9,Planilha1!$B$16,Planilha1!$B$23,Planilha1!$B$30,Planilha1!$B$37,Planilha1!$B$44)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Planilha1!$M$4,Planilha1!$M$11,Planilha1!$M$18,Planilha1!$M$25,Planilha1!$M$32,Planilha1!$M$39,Planilha1!$M$46)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5.3333333333333332E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35433333333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4186666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.7486666666666677</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.017333333333337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000003C-6783-48CC-9102-FAE554ACBD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Planilha1!$B$2,Planilha1!$B$9,Planilha1!$B$16,Planilha1!$B$23,Planilha1!$B$30,Planilha1!$B$37,Planilha1!$B$44)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Planilha1!$M$5,Planilha1!$M$12,Planilha1!$M$19,Planilha1!$M$26,Planilha1!$M$33,Planilha1!$M$40,Planilha1!$M$47)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.7000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25966666666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0573333333333332</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2543333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.034666666666666</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>69.833333333333329</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000003D-6783-48CC-9102-FAE554ACBD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Merge</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Planilha1!$B$2,Planilha1!$B$9,Planilha1!$B$16,Planilha1!$B$23,Planilha1!$B$30,Planilha1!$B$37,Planilha1!$B$44)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Planilha1!$M$6,Planilha1!$M$13,Planilha1!$M$20,Planilha1!$M$27,Planilha1!$M$34,Planilha1!$M$41,Planilha1!$M$48)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6666666666666664E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.3333333333333332E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1333333333333334E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.466666666666667E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000003E-6783-48CC-9102-FAE554ACBD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Planilha1!$B$2,Planilha1!$B$9,Planilha1!$B$16,Planilha1!$B$23,Planilha1!$B$30,Planilha1!$B$37,Planilha1!$B$44)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Planilha1!$M$7,Planilha1!$M$14,Planilha1!$M$21,Planilha1!$M$28,Planilha1!$M$35,Planilha1!$M$42,Planilha1!$M$49)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0000000000000005E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.6666666666666671E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000003F-6783-48CC-9102-FAE554ACBD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Select com bubble</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showVal val="1"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Planilha1!$B$2,Planilha1!$B$9,Planilha1!$B$16,Planilha1!$B$23,Planilha1!$B$30,Planilha1!$B$37,Planilha1!$B$44)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Planilha1!$M$8,Planilha1!$M$15,Planilha1!$M$22,Planilha1!$M$29,Planilha1!$M$36,Planilha1!$M$43,Planilha1!$M$50)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.6333333333333335E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0666666666666665E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70233333333333325</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.778</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.111333333333334</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44.664999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000040-6783-48CC-9102-FAE554ACBD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="159095424"/>
+        <c:axId val="159376896"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="159095424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Quantidade de elementos no vetor</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="159376896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="159376896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Tempo gasto no processamento (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="159095424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2762,6 +4910,66 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>27215</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>8164</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>44532</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>13607</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>606878</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>71746</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2808,7 +5016,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2843,7 +5051,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3020,26 +5228,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3059,7 +5267,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="B2" s="1">
         <v>2000</v>
       </c>
@@ -3081,7 +5289,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3098,16 +5306,34 @@
         <f>AVERAGE(B3:D3)</f>
         <v>3.0000000000000005E-3</v>
       </c>
-      <c r="I3" t="e">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <f>AVERAGE(F3:H3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M3" t="e">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="L3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="M3">
         <f>AVERAGE(J3:L3)</f>
-        <v>#DIV/0!</v>
+        <v>5.6666666666666671E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3124,16 +5350,34 @@
         <f t="shared" ref="E4:E8" si="0">AVERAGE(B4:D4)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I4" t="e">
+      <c r="F4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I4">
         <f t="shared" ref="I4:I8" si="1">AVERAGE(F4:H4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M4" t="e">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="M4">
         <f t="shared" ref="M4:M8" si="2">AVERAGE(J4:L4)</f>
-        <v>#DIV/0!</v>
+        <v>5.3333333333333332E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -3150,16 +5394,34 @@
         <f t="shared" si="0"/>
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="I5" t="e">
+      <c r="F5">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G5">
+        <v>1.2E-2</v>
+      </c>
+      <c r="H5">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M5" t="e">
+        <v>1.1666666666666667E-2</v>
+      </c>
+      <c r="J5">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="K5">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="L5">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="M5">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -3176,16 +5438,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" t="e">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M6" t="e">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -3202,16 +5482,34 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" t="e">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M7" t="e">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -3228,16 +5526,34 @@
         <f t="shared" si="0"/>
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="I8" t="e">
+      <c r="F8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M8" t="e">
+        <v>5.3333333333333332E-3</v>
+      </c>
+      <c r="J8">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="K8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>1.6333333333333335E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="B9" s="1">
         <f>B2*2</f>
         <v>4000</v>
@@ -3260,7 +5576,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -3277,16 +5593,34 @@
         <f>AVERAGE(B10:D10)</f>
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="I10" t="e">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
         <f>AVERAGE(F10:H10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M10" t="e">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>2.3E-2</v>
+      </c>
+      <c r="K10">
+        <v>2.3E-2</v>
+      </c>
+      <c r="L10">
+        <v>2.4E-2</v>
+      </c>
+      <c r="M10">
         <f>AVERAGE(J10:L10)</f>
-        <v>#DIV/0!</v>
+        <v>2.3333333333333334E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -3303,16 +5637,34 @@
         <f t="shared" ref="E11:E15" si="3">AVERAGE(B11:D11)</f>
         <v>2.4666666666666667E-2</v>
       </c>
-      <c r="I11" t="e">
+      <c r="F11">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="G11">
+        <v>2.4E-2</v>
+      </c>
+      <c r="H11">
+        <v>2.4E-2</v>
+      </c>
+      <c r="I11">
         <f t="shared" ref="I11:I15" si="4">AVERAGE(F11:H11)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M11" t="e">
+        <v>2.3000000000000003E-2</v>
+      </c>
+      <c r="J11">
+        <v>2.3E-2</v>
+      </c>
+      <c r="K11">
+        <v>2.3E-2</v>
+      </c>
+      <c r="L11">
+        <v>2.3E-2</v>
+      </c>
+      <c r="M11">
         <f t="shared" ref="M11:M15" si="5">AVERAGE(J11:L11)</f>
-        <v>#DIV/0!</v>
+        <v>2.3000000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -3329,16 +5681,34 @@
         <f t="shared" si="3"/>
         <v>7.5333333333333322E-2</v>
       </c>
-      <c r="I12" t="e">
+      <c r="F12">
+        <v>0.05</v>
+      </c>
+      <c r="G12">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="H12">
+        <v>0.05</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M12" t="e">
+        <v>4.9666666666666671E-2</v>
+      </c>
+      <c r="J12">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="K12">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="L12">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>6.6666666666666666E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -3355,16 +5725,34 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I13" t="e">
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M13" t="e">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>2E-3</v>
+      </c>
+      <c r="M13">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>6.6666666666666664E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -3381,16 +5769,34 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I14" t="e">
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M14" t="e">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -3407,16 +5813,34 @@
         <f t="shared" si="3"/>
         <v>5.8666666666666666E-2</v>
       </c>
-      <c r="I15" t="e">
+      <c r="F15">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="G15">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H15">
+        <v>2.3E-2</v>
+      </c>
+      <c r="I15">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M15" t="e">
+        <v>2.2333333333333334E-2</v>
+      </c>
+      <c r="J15">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="K15">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="L15">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="M15">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>5.0666666666666665E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="B16" s="1">
         <f>B9*2</f>
         <v>8000</v>
@@ -3439,7 +5863,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -3456,16 +5880,34 @@
         <f>AVERAGE(B17:D17)</f>
         <v>5.1333333333333335E-2</v>
       </c>
-      <c r="I17" t="e">
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
         <f>AVERAGE(F17:H17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M17" t="e">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0.09</v>
+      </c>
+      <c r="K17">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="L17">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="M17">
         <f>AVERAGE(J17:L17)</f>
-        <v>#DIV/0!</v>
+        <v>9.1000000000000011E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -3482,16 +5924,34 @@
         <f t="shared" ref="E18:E22" si="6">AVERAGE(B18:D18)</f>
         <v>8.7000000000000008E-2</v>
       </c>
-      <c r="I18" t="e">
+      <c r="F18">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="G18">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="H18">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="I18">
         <f t="shared" ref="I18:I22" si="7">AVERAGE(F18:H18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M18" t="e">
+        <v>8.8000000000000009E-2</v>
+      </c>
+      <c r="J18">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="K18">
+        <v>0.09</v>
+      </c>
+      <c r="L18">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="M18">
         <f t="shared" ref="M18:M22" si="8">AVERAGE(J18:L18)</f>
-        <v>#DIV/0!</v>
+        <v>8.8333333333333333E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -3508,16 +5968,34 @@
         <f t="shared" si="6"/>
         <v>0.21353333333333335</v>
       </c>
-      <c r="I19" t="e">
+      <c r="F19">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="G19">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="H19">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="I19">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M19" t="e">
+        <v>0.17800000000000002</v>
+      </c>
+      <c r="J19">
+        <v>0.26</v>
+      </c>
+      <c r="K19">
+        <v>0.26</v>
+      </c>
+      <c r="L19">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="M19">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>0.25966666666666666</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -3534,16 +6012,34 @@
         <f t="shared" si="6"/>
         <v>1E-3</v>
       </c>
-      <c r="I20" t="e">
+      <c r="F20">
+        <v>1E-3</v>
+      </c>
+      <c r="G20">
+        <v>1E-3</v>
+      </c>
+      <c r="H20">
+        <v>1E-3</v>
+      </c>
+      <c r="I20">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M20" t="e">
+        <v>1E-3</v>
+      </c>
+      <c r="J20">
+        <v>1E-3</v>
+      </c>
+      <c r="K20">
+        <v>1E-3</v>
+      </c>
+      <c r="L20">
+        <v>1E-3</v>
+      </c>
+      <c r="M20">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>1E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -3560,16 +6056,34 @@
         <f t="shared" si="6"/>
         <v>1E-3</v>
       </c>
-      <c r="I21" t="e">
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M21" t="e">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -3586,16 +6100,34 @@
         <f t="shared" si="6"/>
         <v>0.20933333333333334</v>
       </c>
-      <c r="I22" t="e">
+      <c r="F22">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="G22">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="H22">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M22" t="e">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="J22">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="K22">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="L22">
+        <v>0.17</v>
+      </c>
+      <c r="M22">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>0.17</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="B23" s="1">
         <f>B16*2</f>
         <v>16000</v>
@@ -3618,7 +6150,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -3635,16 +6167,34 @@
         <f>AVERAGE(B24:D24)</f>
         <v>0.19899999999999998</v>
       </c>
-      <c r="I24" t="e">
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
         <f>AVERAGE(F24:H24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M24" t="e">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0.97</v>
+      </c>
+      <c r="K24">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="L24">
+        <v>0.371</v>
+      </c>
+      <c r="M24">
         <f>AVERAGE(J24:L24)</f>
-        <v>#DIV/0!</v>
+        <v>0.56966666666666665</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -3661,16 +6211,34 @@
         <f t="shared" ref="E25:E29" si="9">AVERAGE(B25:D25)</f>
         <v>0.34899999999999998</v>
       </c>
-      <c r="I25" t="e">
+      <c r="F25">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="G25">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="H25">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="I25">
         <f t="shared" ref="I25:I29" si="10">AVERAGE(F25:H25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M25" t="e">
+        <v>0.34766666666666662</v>
+      </c>
+      <c r="J25">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="K25">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="L25">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="M25">
         <f t="shared" ref="M25:M29" si="11">AVERAGE(J25:L25)</f>
-        <v>#DIV/0!</v>
+        <v>0.35433333333333333</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -3687,16 +6255,34 @@
         <f t="shared" si="9"/>
         <v>1.2793333333333334</v>
       </c>
-      <c r="I26" t="e">
+      <c r="F26">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="G26">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="H26">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M26" t="e">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="J26">
+        <v>1.0489999999999999</v>
+      </c>
+      <c r="K26">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="L26">
+        <v>1.0580000000000001</v>
+      </c>
+      <c r="M26">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>1.0573333333333332</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -3713,16 +6299,34 @@
         <f t="shared" si="9"/>
         <v>3.0000000000000005E-3</v>
       </c>
-      <c r="I27" t="e">
+      <c r="F27">
+        <v>2E-3</v>
+      </c>
+      <c r="G27">
+        <v>2E-3</v>
+      </c>
+      <c r="H27">
+        <v>2E-3</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M27" t="e">
+        <v>2E-3</v>
+      </c>
+      <c r="J27">
+        <v>2E-3</v>
+      </c>
+      <c r="K27">
+        <v>2E-3</v>
+      </c>
+      <c r="L27">
+        <v>2E-3</v>
+      </c>
+      <c r="M27">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>2E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -3739,16 +6343,34 @@
         <f t="shared" si="9"/>
         <v>2E-3</v>
       </c>
-      <c r="I28" t="e">
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M28" t="e">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -3765,16 +6387,34 @@
         <f t="shared" si="9"/>
         <v>0.88166666666666671</v>
       </c>
-      <c r="I29" t="e">
+      <c r="F29">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="G29">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="H29">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="I29">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M29" t="e">
+        <v>0.34533333333333333</v>
+      </c>
+      <c r="J29">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="K29">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="L29">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="M29">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0.70233333333333325</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="B30" s="1">
         <f>B23*2</f>
         <v>32000</v>
@@ -3797,7 +6437,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -3814,16 +6454,34 @@
         <f>AVERAGE(B31:D31)</f>
         <v>0.73966666666666681</v>
       </c>
-      <c r="I31" t="e">
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
         <f>AVERAGE(F31:H31)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M31" t="e">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>1.486</v>
+      </c>
+      <c r="K31">
+        <v>1.47</v>
+      </c>
+      <c r="L31">
+        <v>1.4690000000000001</v>
+      </c>
+      <c r="M31">
         <f>AVERAGE(J31:L31)</f>
-        <v>#DIV/0!</v>
+        <v>1.4749999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -3840,16 +6498,34 @@
         <f t="shared" ref="E32:E36" si="12">AVERAGE(B32:D32)</f>
         <v>1.42</v>
       </c>
-      <c r="I32" t="e">
+      <c r="F32">
+        <v>1.389</v>
+      </c>
+      <c r="G32">
+        <v>1.3959999999999999</v>
+      </c>
+      <c r="H32">
+        <v>1.405</v>
+      </c>
+      <c r="I32">
         <f t="shared" ref="I32:I36" si="13">AVERAGE(F32:H32)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M32" t="e">
+        <v>1.3966666666666667</v>
+      </c>
+      <c r="J32">
+        <v>1.4179999999999999</v>
+      </c>
+      <c r="K32">
+        <v>1.417</v>
+      </c>
+      <c r="L32">
+        <v>1.421</v>
+      </c>
+      <c r="M32">
         <f t="shared" ref="M32:M36" si="14">AVERAGE(J32:L32)</f>
-        <v>#DIV/0!</v>
+        <v>1.4186666666666667</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -3866,16 +6542,34 @@
         <f t="shared" si="12"/>
         <v>5.1643333333333334</v>
       </c>
-      <c r="I33" t="e">
+      <c r="F33">
+        <v>2.9039999999999999</v>
+      </c>
+      <c r="G33">
+        <v>2.8940000000000001</v>
+      </c>
+      <c r="H33">
+        <v>2.8839999999999999</v>
+      </c>
+      <c r="I33">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M33" t="e">
+        <v>2.8940000000000001</v>
+      </c>
+      <c r="J33">
+        <v>4.2640000000000002</v>
+      </c>
+      <c r="K33">
+        <v>4.22</v>
+      </c>
+      <c r="L33">
+        <v>4.2789999999999999</v>
+      </c>
+      <c r="M33">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>4.2543333333333333</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -3892,16 +6586,34 @@
         <f t="shared" si="12"/>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="I34" t="e">
+      <c r="F34">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G34">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H34">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I34">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M34" t="e">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J34">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K34">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L34">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="M34">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>5.3333333333333332E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -3918,16 +6630,34 @@
         <f t="shared" si="12"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="I35" t="e">
+      <c r="F35">
+        <v>1E-3</v>
+      </c>
+      <c r="G35">
+        <v>1E-3</v>
+      </c>
+      <c r="H35">
+        <v>1E-3</v>
+      </c>
+      <c r="I35">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M35" t="e">
+        <v>1E-3</v>
+      </c>
+      <c r="J35">
+        <v>1E-3</v>
+      </c>
+      <c r="K35">
+        <v>1E-3</v>
+      </c>
+      <c r="L35">
+        <v>1E-3</v>
+      </c>
+      <c r="M35">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>1E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -3944,16 +6674,34 @@
         <f t="shared" si="12"/>
         <v>3.59</v>
       </c>
-      <c r="I36" t="e">
+      <c r="F36">
+        <v>1.383</v>
+      </c>
+      <c r="G36">
+        <v>1.3839999999999999</v>
+      </c>
+      <c r="H36">
+        <v>1.383</v>
+      </c>
+      <c r="I36">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M36" t="e">
+        <v>1.3833333333333335</v>
+      </c>
+      <c r="J36">
+        <v>2.7869999999999999</v>
+      </c>
+      <c r="K36">
+        <v>2.7610000000000001</v>
+      </c>
+      <c r="L36">
+        <v>2.786</v>
+      </c>
+      <c r="M36">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
+        <v>2.778</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13">
       <c r="B37" s="1">
         <f>B30*2</f>
         <v>64000</v>
@@ -3976,7 +6724,7 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -3993,16 +6741,34 @@
         <f>AVERAGE(B38:D38)</f>
         <v>2.7749999999999999</v>
       </c>
-      <c r="I38" t="e">
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
         <f>AVERAGE(F38:H38)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M38" t="e">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>5.9960000000000004</v>
+      </c>
+      <c r="K38">
+        <v>5.9450000000000003</v>
+      </c>
+      <c r="L38">
+        <v>5.9089999999999998</v>
+      </c>
+      <c r="M38">
         <f>AVERAGE(J38:L38)</f>
-        <v>#DIV/0!</v>
+        <v>5.95</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -4019,16 +6785,34 @@
         <f t="shared" ref="E39:E43" si="15">AVERAGE(B39:D39)</f>
         <v>5.5883333333333338</v>
       </c>
-      <c r="I39" t="e">
+      <c r="F39">
+        <v>5.6230000000000002</v>
+      </c>
+      <c r="G39">
+        <v>5.6150000000000002</v>
+      </c>
+      <c r="H39">
+        <v>5.5720000000000001</v>
+      </c>
+      <c r="I39">
         <f t="shared" ref="I39:I43" si="16">AVERAGE(F39:H39)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M39" t="e">
+        <v>5.6033333333333326</v>
+      </c>
+      <c r="J39">
+        <v>5.7750000000000004</v>
+      </c>
+      <c r="K39">
+        <v>5.7640000000000002</v>
+      </c>
+      <c r="L39">
+        <v>5.7069999999999999</v>
+      </c>
+      <c r="M39">
         <f t="shared" ref="M39:M43" si="17">AVERAGE(J39:L39)</f>
-        <v>#DIV/0!</v>
+        <v>5.7486666666666677</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -4045,16 +6829,34 @@
         <f t="shared" si="15"/>
         <v>20.272000000000002</v>
       </c>
-      <c r="I40" t="e">
+      <c r="F40">
+        <v>11.356</v>
+      </c>
+      <c r="G40">
+        <v>11.414999999999999</v>
+      </c>
+      <c r="H40">
+        <v>11.33</v>
+      </c>
+      <c r="I40">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M40" t="e">
+        <v>11.366999999999999</v>
+      </c>
+      <c r="J40">
+        <v>17.128</v>
+      </c>
+      <c r="K40">
+        <v>16.923999999999999</v>
+      </c>
+      <c r="L40">
+        <v>17.052</v>
+      </c>
+      <c r="M40">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>17.034666666666666</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -4071,16 +6873,34 @@
         <f t="shared" si="15"/>
         <v>1.7666666666666667E-2</v>
       </c>
-      <c r="I41" t="e">
+      <c r="F41">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G41">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="H41">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I41">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M41" t="e">
+        <v>1.1333333333333334E-2</v>
+      </c>
+      <c r="J41">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="K41">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="L41">
+        <v>1.2E-2</v>
+      </c>
+      <c r="M41">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>1.1333333333333334E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -4097,16 +6917,34 @@
         <f t="shared" si="15"/>
         <v>0.01</v>
       </c>
-      <c r="I42" t="e">
+      <c r="F42">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G42">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H42">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I42">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M42" t="e">
+        <v>3.0000000000000005E-3</v>
+      </c>
+      <c r="J42">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K42">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L42">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="M42">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>3.0000000000000005E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -4123,16 +6961,34 @@
         <f t="shared" si="15"/>
         <v>13.960333333333333</v>
       </c>
-      <c r="I43" t="e">
+      <c r="F43">
+        <v>5.585</v>
+      </c>
+      <c r="G43">
+        <v>5.5540000000000003</v>
+      </c>
+      <c r="H43">
+        <v>5.5410000000000004</v>
+      </c>
+      <c r="I43">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M43" t="e">
+        <v>5.56</v>
+      </c>
+      <c r="J43">
+        <v>11.146000000000001</v>
+      </c>
+      <c r="K43">
+        <v>11.106</v>
+      </c>
+      <c r="L43">
+        <v>11.082000000000001</v>
+      </c>
+      <c r="M43">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>11.111333333333334</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13">
       <c r="B44" s="1">
         <f>B37*2</f>
         <v>128000</v>
@@ -4155,7 +7011,7 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -4172,16 +7028,34 @@
         <f>AVERAGE(B45:D45)</f>
         <v>11.435333333333332</v>
       </c>
-      <c r="I45" t="e">
+      <c r="F45">
+        <v>1E-3</v>
+      </c>
+      <c r="G45">
+        <v>1E-3</v>
+      </c>
+      <c r="H45">
+        <v>1E-3</v>
+      </c>
+      <c r="I45">
         <f>AVERAGE(F45:H45)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M45" t="e">
+        <v>1E-3</v>
+      </c>
+      <c r="J45">
+        <v>23.856999999999999</v>
+      </c>
+      <c r="K45">
+        <v>23.952000000000002</v>
+      </c>
+      <c r="L45">
+        <v>23.972000000000001</v>
+      </c>
+      <c r="M45">
         <f>AVERAGE(J45:L45)</f>
-        <v>#DIV/0!</v>
+        <v>23.927000000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -4198,16 +7072,34 @@
         <f t="shared" ref="E46:E50" si="18">AVERAGE(B46:D46)</f>
         <v>22.591666666666669</v>
       </c>
-      <c r="I46" t="e">
+      <c r="F46">
+        <v>22.640999999999998</v>
+      </c>
+      <c r="G46">
+        <v>22.532</v>
+      </c>
+      <c r="H46">
+        <v>22.530999999999999</v>
+      </c>
+      <c r="I46">
         <f t="shared" ref="I46:I50" si="19">AVERAGE(F46:H46)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M46" t="e">
+        <v>22.568000000000001</v>
+      </c>
+      <c r="J46">
+        <v>23.100999999999999</v>
+      </c>
+      <c r="K46">
+        <v>22.962</v>
+      </c>
+      <c r="L46">
+        <v>22.989000000000001</v>
+      </c>
+      <c r="M46">
         <f t="shared" ref="M46:M50" si="20">AVERAGE(J46:L46)</f>
-        <v>#DIV/0!</v>
+        <v>23.017333333333337</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -4224,16 +7116,34 @@
         <f t="shared" si="18"/>
         <v>81.22433333333332</v>
       </c>
-      <c r="I47" t="e">
+      <c r="F47">
+        <v>46.206000000000003</v>
+      </c>
+      <c r="G47">
+        <v>46.174999999999997</v>
+      </c>
+      <c r="H47">
+        <v>46.155000000000001</v>
+      </c>
+      <c r="I47">
         <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M47" t="e">
+        <v>46.178666666666665</v>
+      </c>
+      <c r="J47">
+        <v>69.909000000000006</v>
+      </c>
+      <c r="K47">
+        <v>69.734999999999999</v>
+      </c>
+      <c r="L47">
+        <v>69.855999999999995</v>
+      </c>
+      <c r="M47">
         <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
+        <v>69.833333333333329</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -4250,16 +7160,34 @@
         <f t="shared" si="18"/>
         <v>3.7333333333333329E-2</v>
       </c>
-      <c r="I48" t="e">
+      <c r="F48">
+        <v>2.4E-2</v>
+      </c>
+      <c r="G48">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H48">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I48">
         <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M48" t="e">
+        <v>2.466666666666667E-2</v>
+      </c>
+      <c r="J48">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K48">
+        <v>2.4E-2</v>
+      </c>
+      <c r="L48">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M48">
         <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
+        <v>2.466666666666667E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -4276,16 +7204,34 @@
         <f t="shared" si="18"/>
         <v>2.1666666666666667E-2</v>
       </c>
-      <c r="I49" t="e">
+      <c r="F49">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G49">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="H49">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I49">
         <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M49" t="e">
+        <v>6.000000000000001E-3</v>
+      </c>
+      <c r="J49">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K49">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="L49">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="M49">
         <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
+        <v>6.6666666666666671E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -4302,41 +7248,59 @@
         <f t="shared" si="18"/>
         <v>56.147333333333336</v>
       </c>
-      <c r="I50" t="e">
+      <c r="F50">
+        <v>22.245000000000001</v>
+      </c>
+      <c r="G50">
+        <v>22.213999999999999</v>
+      </c>
+      <c r="H50">
+        <v>22.257999999999999</v>
+      </c>
+      <c r="I50">
         <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M50" t="e">
+        <v>22.239000000000001</v>
+      </c>
+      <c r="J50">
+        <v>44.844999999999999</v>
+      </c>
+      <c r="K50">
+        <v>44.545999999999999</v>
+      </c>
+      <c r="L50">
+        <v>44.603999999999999</v>
+      </c>
+      <c r="M50">
         <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
+        <v>44.664999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="J30:M30"/>
     <mergeCell ref="B37:E37"/>
     <mergeCell ref="F37:I37"/>
     <mergeCell ref="J37:M37"/>
     <mergeCell ref="B44:E44"/>
     <mergeCell ref="F44:I44"/>
     <mergeCell ref="J44:M44"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>